<commit_message>
before changing the 3D skeleton, c++
</commit_message>
<xml_diff>
--- a/Documents/temps.xlsx
+++ b/Documents/temps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptitg\Documents\Thesis-animal-animation\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1867204B-5543-483F-94B2-FBE71F92B818}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B893DE-4019-4722-BE42-27BF8C1789DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4620" yWindow="-10395" windowWidth="16875" windowHeight="10530" xr2:uid="{454B0C08-6FB4-4BA4-8296-F953A4E05736}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="16875" windowHeight="10522" xr2:uid="{454B0C08-6FB4-4BA4-8296-F953A4E05736}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>install opencv</t>
   </si>
@@ -114,6 +114,30 @@
   </si>
   <si>
     <t>discussion</t>
+  </si>
+  <si>
+    <t>Lun 03 Feb</t>
+  </si>
+  <si>
+    <t>3D  morphable skeleton</t>
+  </si>
+  <si>
+    <t>Mar 04 Feb</t>
+  </si>
+  <si>
+    <t>Mer 05 Feb</t>
+  </si>
+  <si>
+    <t>Jeu 06 Feb</t>
+  </si>
+  <si>
+    <t>quaternion</t>
+  </si>
+  <si>
+    <t>Ven 07 Feb</t>
+  </si>
+  <si>
+    <t>3D skeleton</t>
   </si>
 </sst>
 </file>
@@ -149,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,6 +188,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2325,8 +2367,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A3:AT50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:T3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2339,7 +2381,9 @@
     <col min="6" max="6" width="11.06640625" style="1" customWidth="1"/>
     <col min="7" max="15" width="10.6640625" style="1"/>
     <col min="16" max="16" width="12.6640625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.6640625" style="1"/>
+    <col min="17" max="20" width="10.6640625" style="1"/>
+    <col min="21" max="21" width="14.265625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:46" x14ac:dyDescent="0.45">
@@ -2349,24 +2393,24 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16"/>
+      <c r="E3" s="22"/>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16" t="s">
+      <c r="I3" s="22"/>
+      <c r="J3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="16"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2376,18 +2420,33 @@
       <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="16"/>
+      <c r="P3" s="22"/>
       <c r="Q3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="R3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:46" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
@@ -2446,6 +2505,21 @@
       </c>
       <c r="T5" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.45">
@@ -2506,6 +2580,18 @@
       <c r="T6" s="14">
         <v>6.25E-2</v>
       </c>
+      <c r="U6" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V6" s="17">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="W6" s="18">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="X6" s="19">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.45">
       <c r="B7" s="3">
@@ -2543,6 +2629,18 @@
       </c>
       <c r="Q7" s="11">
         <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="U7" s="16">
+        <v>0.14027777777777778</v>
+      </c>
+      <c r="V7" s="17">
+        <v>0.22569444444444445</v>
+      </c>
+      <c r="W7" s="19">
+        <v>0.11597222222222221</v>
+      </c>
+      <c r="X7" s="20">
+        <v>0.1451388888888889</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.45">
@@ -2652,19 +2750,19 @@
       </c>
       <c r="U10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.18194444444444444</v>
       </c>
       <c r="V10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.24652777777777779</v>
       </c>
       <c r="W10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16805555555555554</v>
       </c>
       <c r="X10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.18680555555555556</v>
       </c>
       <c r="Y10" s="11">
         <f t="shared" si="1"/>
@@ -2770,11 +2868,11 @@
         <f>C10</f>
         <v>0.17916666666666667</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="21">
         <f>SUM(D10:E10)</f>
         <v>0.2388888888888889</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="3">
         <f>F10</f>
         <v>0.2361111111111111</v>
@@ -2783,16 +2881,16 @@
         <f t="shared" ref="G12:L12" si="2">G10</f>
         <v>0.25416666666666665</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="21">
         <f>SUM(H10:I10)</f>
         <v>0.2326388888888889</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="15">
+      <c r="I12" s="22"/>
+      <c r="J12" s="21">
         <f>SUM(J10:K10)</f>
         <v>0.23541666666666666</v>
       </c>
-      <c r="K12" s="16"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="3">
         <f t="shared" si="2"/>
         <v>0.17916666666666664</v>
@@ -2805,36 +2903,36 @@
         <f t="shared" si="3"/>
         <v>0.2326388888888889</v>
       </c>
-      <c r="O12" s="15">
+      <c r="O12" s="21">
         <f>SUM(O10:P10)</f>
         <v>0.19583333333333333</v>
       </c>
-      <c r="P12" s="16"/>
+      <c r="P12" s="22"/>
       <c r="Q12" s="11">
         <f t="shared" si="3"/>
         <v>0.20069444444444445</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="21">
         <f>SUM(R10:T10)</f>
         <v>0.15277777777777779</v>
       </c>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
       <c r="U12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.18194444444444444</v>
       </c>
       <c r="V12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.24652777777777779</v>
       </c>
       <c r="W12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.16805555555555554</v>
       </c>
       <c r="X12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.18680555555555556</v>
       </c>
       <c r="Y12" s="11">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
finish optimization lower part of legs
</commit_message>
<xml_diff>
--- a/Documents/temps.xlsx
+++ b/Documents/temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptitg\Documents\Thesis-animal-animation\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91220EEB-EAF6-4EFA-AD01-91939D1C718A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720E02E-AC50-49E8-8D76-15039B0D9864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2205" yWindow="2205" windowWidth="16875" windowHeight="10523" xr2:uid="{454B0C08-6FB4-4BA4-8296-F953A4E05736}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>install opencv</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>angle constraints</t>
+  </si>
+  <si>
+    <t>optimisation</t>
+  </si>
+  <si>
+    <t>Ven 14 Feb</t>
+  </si>
+  <si>
+    <t>Lun 17 Feb</t>
   </si>
 </sst>
 </file>
@@ -197,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,6 +221,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2409,8 +2433,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A3:AT50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+    <sheetView tabSelected="1" topLeftCell="AB2" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2435,24 +2459,24 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="28"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28" t="s">
+      <c r="I3" s="33"/>
+      <c r="J3" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="28"/>
+      <c r="K3" s="33"/>
       <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2462,18 +2486,18 @@
       <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="27" t="s">
+      <c r="O3" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="28"/>
+      <c r="P3" s="33"/>
       <c r="Q3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="28" t="s">
+      <c r="R3" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
       <c r="U3" s="1" t="s">
         <v>27</v>
       </c>
@@ -2498,8 +2522,15 @@
       <c r="AB3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AC3" s="33" t="s">
         <v>41</v>
+      </c>
+      <c r="AD3" s="33"/>
+      <c r="AE3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:46" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2587,6 +2618,15 @@
       <c r="AC5" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="AD5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.45">
       <c r="B6" s="3">
@@ -2670,6 +2710,18 @@
       <c r="AB6" s="25">
         <v>5.5555555555555552E-2</v>
       </c>
+      <c r="AC6" s="27">
+        <v>5.4166666666666669E-2</v>
+      </c>
+      <c r="AD6" s="28">
+        <v>0.125</v>
+      </c>
+      <c r="AE6" s="28">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AF6" s="30">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.45">
       <c r="B7" s="3">
@@ -2731,6 +2783,12 @@
       </c>
       <c r="AB7" s="26">
         <v>0.17847222222222223</v>
+      </c>
+      <c r="AE7" s="29">
+        <v>0.14166666666666666</v>
+      </c>
+      <c r="AF7" s="31">
+        <v>0.18402777777777779</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.45">
@@ -2872,19 +2930,19 @@
       </c>
       <c r="AC10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.4166666666666669E-2</v>
       </c>
       <c r="AD10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="AE10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.18333333333333332</v>
       </c>
       <c r="AF10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.22569444444444445</v>
       </c>
       <c r="AG10" s="11">
         <f t="shared" si="1"/>
@@ -2958,11 +3016,11 @@
         <f>C10</f>
         <v>0.17916666666666667</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="32">
         <f>SUM(D10:E10)</f>
         <v>0.2388888888888889</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="3">
         <f>F10</f>
         <v>0.2361111111111111</v>
@@ -2971,16 +3029,16 @@
         <f t="shared" ref="G12:L12" si="2">G10</f>
         <v>0.25416666666666665</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="32">
         <f>SUM(H10:I10)</f>
         <v>0.2326388888888889</v>
       </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="27">
+      <c r="I12" s="33"/>
+      <c r="J12" s="32">
         <f>SUM(J10:K10)</f>
         <v>0.23541666666666666</v>
       </c>
-      <c r="K12" s="28"/>
+      <c r="K12" s="33"/>
       <c r="L12" s="3">
         <f t="shared" si="2"/>
         <v>0.17916666666666664</v>
@@ -2993,21 +3051,21 @@
         <f t="shared" si="3"/>
         <v>0.2326388888888889</v>
       </c>
-      <c r="O12" s="27">
+      <c r="O12" s="32">
         <f>SUM(O10:P10)</f>
         <v>0.19583333333333333</v>
       </c>
-      <c r="P12" s="28"/>
+      <c r="P12" s="33"/>
       <c r="Q12" s="11">
         <f t="shared" si="3"/>
         <v>0.20069444444444445</v>
       </c>
-      <c r="R12" s="27">
+      <c r="R12" s="32">
         <f>SUM(R10:T10)</f>
         <v>0.15277777777777779</v>
       </c>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
       <c r="U12" s="11">
         <f t="shared" si="3"/>
         <v>0.18194444444444444</v>
@@ -3040,21 +3098,18 @@
         <f t="shared" si="3"/>
         <v>0.23402777777777778</v>
       </c>
-      <c r="AC12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="AC12" s="32">
+        <f>SUM(AC10:AD10)</f>
+        <v>0.17916666666666667</v>
+      </c>
+      <c r="AD12" s="33"/>
       <c r="AE12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.18333333333333332</v>
       </c>
       <c r="AF12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.22569444444444445</v>
       </c>
       <c r="AG12" s="11">
         <f t="shared" si="3"/>
@@ -3113,6 +3168,9 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="B13" s="28"/>
+    </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.45">
       <c r="B14" s="3"/>
     </row>
@@ -3233,17 +3291,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O3:P3"/>
+  <mergeCells count="12">
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
higher part of legs
</commit_message>
<xml_diff>
--- a/Documents/temps.xlsx
+++ b/Documents/temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptitg\Documents\Thesis-animal-animation\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720E02E-AC50-49E8-8D76-15039B0D9864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B1C42F-A8C0-428A-809A-552F849EADDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="16875" windowHeight="10523" xr2:uid="{454B0C08-6FB4-4BA4-8296-F953A4E05736}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{454B0C08-6FB4-4BA4-8296-F953A4E05736}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>install opencv</t>
   </si>
@@ -171,6 +171,21 @@
   </si>
   <si>
     <t>Lun 17 Feb</t>
+  </si>
+  <si>
+    <t>Mar 18 Feb</t>
+  </si>
+  <si>
+    <t>higher legs</t>
+  </si>
+  <si>
+    <t>Mer 19 Feb</t>
+  </si>
+  <si>
+    <t>adapte to other images</t>
+  </si>
+  <si>
+    <t>Jeu 20 Feb</t>
   </si>
 </sst>
 </file>
@@ -206,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -221,6 +236,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2434,7 +2461,7 @@
   <dimension ref="A3:AT50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AB2" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+      <selection activeCell="AI8" sqref="AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2449,7 +2476,9 @@
     <col min="16" max="16" width="12.6640625" style="1" customWidth="1"/>
     <col min="17" max="20" width="10.6640625" style="1"/>
     <col min="21" max="21" width="14.265625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.6640625" style="1"/>
+    <col min="22" max="33" width="10.6640625" style="1"/>
+    <col min="34" max="34" width="12.265625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:46" x14ac:dyDescent="0.45">
@@ -2459,24 +2488,24 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="33"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33" t="s">
+      <c r="I3" s="37"/>
+      <c r="J3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="33"/>
+      <c r="K3" s="37"/>
       <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2486,18 +2515,18 @@
       <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="32" t="s">
+      <c r="O3" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="33"/>
+      <c r="P3" s="37"/>
       <c r="Q3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="33" t="s">
+      <c r="R3" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
       <c r="U3" s="1" t="s">
         <v>27</v>
       </c>
@@ -2522,15 +2551,24 @@
       <c r="AB3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="AD3" s="33"/>
+      <c r="AD3" s="37"/>
       <c r="AE3" s="1" t="s">
         <v>44</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:46" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2627,6 +2665,15 @@
       <c r="AF5" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="AG5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.45">
       <c r="B6" s="3">
@@ -2722,6 +2769,15 @@
       <c r="AF6" s="30">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="AG6" s="32">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AH6" s="34">
+        <v>3.125E-2</v>
+      </c>
+      <c r="AI6" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.45">
       <c r="B7" s="3">
@@ -2789,6 +2845,15 @@
       </c>
       <c r="AF7" s="31">
         <v>0.18402777777777779</v>
+      </c>
+      <c r="AG7" s="33">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="AH7" s="34">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="AI7" s="35">
+        <v>0.13541666666666666</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.45">
@@ -2946,15 +3011,15 @@
       </c>
       <c r="AG10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.15277777777777776</v>
       </c>
       <c r="AH10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="AI10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.17708333333333331</v>
       </c>
       <c r="AJ10" s="11">
         <f t="shared" si="1"/>
@@ -3016,11 +3081,11 @@
         <f>C10</f>
         <v>0.17916666666666667</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="36">
         <f>SUM(D10:E10)</f>
         <v>0.2388888888888889</v>
       </c>
-      <c r="E12" s="33"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="3">
         <f>F10</f>
         <v>0.2361111111111111</v>
@@ -3029,16 +3094,16 @@
         <f t="shared" ref="G12:L12" si="2">G10</f>
         <v>0.25416666666666665</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="36">
         <f>SUM(H10:I10)</f>
         <v>0.2326388888888889</v>
       </c>
-      <c r="I12" s="33"/>
-      <c r="J12" s="32">
+      <c r="I12" s="37"/>
+      <c r="J12" s="36">
         <f>SUM(J10:K10)</f>
         <v>0.23541666666666666</v>
       </c>
-      <c r="K12" s="33"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="3">
         <f t="shared" si="2"/>
         <v>0.17916666666666664</v>
@@ -3051,21 +3116,21 @@
         <f t="shared" si="3"/>
         <v>0.2326388888888889</v>
       </c>
-      <c r="O12" s="32">
+      <c r="O12" s="36">
         <f>SUM(O10:P10)</f>
         <v>0.19583333333333333</v>
       </c>
-      <c r="P12" s="33"/>
+      <c r="P12" s="37"/>
       <c r="Q12" s="11">
         <f t="shared" si="3"/>
         <v>0.20069444444444445</v>
       </c>
-      <c r="R12" s="32">
+      <c r="R12" s="36">
         <f>SUM(R10:T10)</f>
         <v>0.15277777777777779</v>
       </c>
-      <c r="S12" s="32"/>
-      <c r="T12" s="32"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
       <c r="U12" s="11">
         <f t="shared" si="3"/>
         <v>0.18194444444444444</v>
@@ -3098,11 +3163,11 @@
         <f t="shared" si="3"/>
         <v>0.23402777777777778</v>
       </c>
-      <c r="AC12" s="32">
+      <c r="AC12" s="36">
         <f>SUM(AC10:AD10)</f>
         <v>0.17916666666666667</v>
       </c>
-      <c r="AD12" s="33"/>
+      <c r="AD12" s="37"/>
       <c r="AE12" s="11">
         <f t="shared" si="3"/>
         <v>0.18333333333333332</v>
@@ -3113,15 +3178,15 @@
       </c>
       <c r="AG12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.15277777777777776</v>
       </c>
       <c r="AH12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="AI12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.17708333333333331</v>
       </c>
       <c r="AJ12" s="11">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
just before animation, still one leg not wormaria is the best king
</commit_message>
<xml_diff>
--- a/Documents/temps.xlsx
+++ b/Documents/temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptitg\Documents\Thesis-animal-animation\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B1C42F-A8C0-428A-809A-552F849EADDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18CD404-88A8-4C7B-A74D-1F9AF83AA3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{454B0C08-6FB4-4BA4-8296-F953A4E05736}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="16875" windowHeight="10522" xr2:uid="{454B0C08-6FB4-4BA4-8296-F953A4E05736}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>install opencv</t>
   </si>
@@ -186,6 +186,15 @@
   </si>
   <si>
     <t>Jeu 20 Feb</t>
+  </si>
+  <si>
+    <t>Ven 21 Feb</t>
+  </si>
+  <si>
+    <t>Lun 24 Feb</t>
+  </si>
+  <si>
+    <t>Distance transform</t>
   </si>
 </sst>
 </file>
@@ -221,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,6 +245,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2461,7 +2476,7 @@
   <dimension ref="A3:AT50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AB2" workbookViewId="0">
-      <selection activeCell="AI8" sqref="AI8"/>
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2488,24 +2503,24 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37" t="s">
+      <c r="I3" s="39"/>
+      <c r="J3" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="37"/>
+      <c r="K3" s="39"/>
       <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2515,18 +2530,18 @@
       <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="O3" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="37"/>
+      <c r="P3" s="39"/>
       <c r="Q3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="37" t="s">
+      <c r="R3" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
       <c r="U3" s="1" t="s">
         <v>27</v>
       </c>
@@ -2551,10 +2566,10 @@
       <c r="AB3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="37" t="s">
+      <c r="AC3" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="AD3" s="37"/>
+      <c r="AD3" s="39"/>
       <c r="AE3" s="1" t="s">
         <v>44</v>
       </c>
@@ -2569,6 +2584,12 @@
       </c>
       <c r="AI3" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:46" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2674,6 +2695,12 @@
       <c r="AI5" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="AJ5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.45">
       <c r="B6" s="3">
@@ -2778,6 +2805,12 @@
       <c r="AI6" s="34">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="AJ6" s="36">
+        <v>3.125E-2</v>
+      </c>
+      <c r="AK6" s="37">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.45">
       <c r="B7" s="3">
@@ -2854,6 +2887,12 @@
       </c>
       <c r="AI7" s="35">
         <v>0.13541666666666666</v>
+      </c>
+      <c r="AJ7" s="36">
+        <v>0.125</v>
+      </c>
+      <c r="AK7" s="37">
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.45">
@@ -3023,11 +3062,11 @@
       </c>
       <c r="AJ10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.15625</v>
       </c>
       <c r="AK10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.10416666666666666</v>
       </c>
       <c r="AL10" s="11">
         <f t="shared" si="1"/>
@@ -3081,11 +3120,11 @@
         <f>C10</f>
         <v>0.17916666666666667</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="38">
         <f>SUM(D10:E10)</f>
         <v>0.2388888888888889</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="3">
         <f>F10</f>
         <v>0.2361111111111111</v>
@@ -3094,16 +3133,16 @@
         <f t="shared" ref="G12:L12" si="2">G10</f>
         <v>0.25416666666666665</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="38">
         <f>SUM(H10:I10)</f>
         <v>0.2326388888888889</v>
       </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="36">
+      <c r="I12" s="39"/>
+      <c r="J12" s="38">
         <f>SUM(J10:K10)</f>
         <v>0.23541666666666666</v>
       </c>
-      <c r="K12" s="37"/>
+      <c r="K12" s="39"/>
       <c r="L12" s="3">
         <f t="shared" si="2"/>
         <v>0.17916666666666664</v>
@@ -3116,21 +3155,21 @@
         <f t="shared" si="3"/>
         <v>0.2326388888888889</v>
       </c>
-      <c r="O12" s="36">
+      <c r="O12" s="38">
         <f>SUM(O10:P10)</f>
         <v>0.19583333333333333</v>
       </c>
-      <c r="P12" s="37"/>
+      <c r="P12" s="39"/>
       <c r="Q12" s="11">
         <f t="shared" si="3"/>
         <v>0.20069444444444445</v>
       </c>
-      <c r="R12" s="36">
+      <c r="R12" s="38">
         <f>SUM(R10:T10)</f>
         <v>0.15277777777777779</v>
       </c>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
+      <c r="S12" s="38"/>
+      <c r="T12" s="38"/>
       <c r="U12" s="11">
         <f t="shared" si="3"/>
         <v>0.18194444444444444</v>
@@ -3163,11 +3202,11 @@
         <f t="shared" si="3"/>
         <v>0.23402777777777778</v>
       </c>
-      <c r="AC12" s="36">
+      <c r="AC12" s="38">
         <f>SUM(AC10:AD10)</f>
         <v>0.17916666666666667</v>
       </c>
-      <c r="AD12" s="37"/>
+      <c r="AD12" s="39"/>
       <c r="AE12" s="11">
         <f t="shared" si="3"/>
         <v>0.18333333333333332</v>
@@ -3190,11 +3229,11 @@
       </c>
       <c r="AJ12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.15625</v>
       </c>
       <c r="AK12" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.10416666666666666</v>
       </c>
       <c r="AL12" s="11">
         <f t="shared" si="3"/>

</xml_diff>